<commit_message>
Helper to run all at once
</commit_message>
<xml_diff>
--- a/code2code.xlsx
+++ b/code2code.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbortolo/work/3_projects/3_BAR/debug_BD/BeamDyn_CpLambda/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\BAR-Local\BeamDyn\BeamDyn_CpLambda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4DE101C3-ED62-AB4C-AB38-DDB4B7FC7C26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B258CB4D-1C6D-4845-B99D-5AF1968C7A6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39560" yWindow="4060" windowWidth="28040" windowHeight="17540"/>
+    <workbookView xWindow="1380" yWindow="-120" windowWidth="27540" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tiploads2" sheetId="1" r:id="rId1"/>
     <sheet name="tiploads3" sheetId="2" r:id="rId2"/>
     <sheet name="tiploads4" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -51,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -5096,21 +5107,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.375" customWidth="1"/>
+    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5139,7 +5150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200000</v>
       </c>
@@ -5170,7 +5181,7 @@
         <v>-1.32312425987368E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>500000</v>
       </c>
@@ -5201,7 +5212,7 @@
         <v>-8.0897077519159297E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000000</v>
       </c>
@@ -5232,7 +5243,7 @@
         <v>-0.30067778834619502</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1500000</v>
       </c>
@@ -5263,7 +5274,7 @@
         <v>-0.60830733147520799</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2000000</v>
       </c>
@@ -5294,7 +5305,7 @@
         <v>-0.95423492285865597</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4000000</v>
       </c>
@@ -5325,7 +5336,7 @@
         <v>-2.24507828347397</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5000000</v>
       </c>
@@ -5356,7 +5367,7 @@
         <v>-2.7516289157643099</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8000000</v>
       </c>
@@ -5387,7 +5398,7 @@
         <v>-3.8308370988538298</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10000000</v>
       </c>
@@ -5425,19 +5436,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5466,7 +5477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>100000</v>
       </c>
@@ -5484,7 +5495,7 @@
         <v>-3.7162143890043402E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>200000</v>
       </c>
@@ -5502,7 +5513,7 @@
         <v>-0.148246062720502</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>300000</v>
       </c>
@@ -5520,7 +5531,7 @@
         <v>-0.332058297522067</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>400000</v>
       </c>
@@ -5538,7 +5549,7 @@
         <v>-0.58665563720094804</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>500000</v>
       </c>
@@ -5556,7 +5567,7 @@
         <v>-0.90941046581797003</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1000000</v>
       </c>
@@ -5574,7 +5585,7 @@
         <v>-3.4173409207288401</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2000000</v>
       </c>
@@ -5599,16 +5610,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5637,7 +5648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -5655,7 +5666,7 @@
         <v>-0.129684284322237</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -5673,7 +5684,7 @@
         <v>-0.51489670994790504</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3000</v>
       </c>
@@ -5691,7 +5702,7 @@
         <v>-1.1444704536519701</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4000</v>
       </c>
@@ -5709,7 +5720,7 @@
         <v>-2.0009096524932901</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5000</v>
       </c>

</xml_diff>